<commit_message>
Added Acceptance Test pdf and Updated Burndown Chart
</commit_message>
<xml_diff>
--- a/documentation/BurndownChartExcel.xlsx
+++ b/documentation/BurndownChartExcel.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
   <si>
     <t>DAY1</t>
   </si>
@@ -249,6 +249,9 @@
   </si>
   <si>
     <t>DAY71</t>
+  </si>
+  <si>
+    <t>DAY72</t>
   </si>
 </sst>
 </file>
@@ -767,6 +770,27 @@
                 <c:pt idx="52">
                   <c:v>0</c:v>
                 </c:pt>
+                <c:pt idx="53">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>3</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -785,8 +809,8 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="219"/>
-        <c:axId val="439814576"/>
-        <c:axId val="439806960"/>
+        <c:axId val="-1263664048"/>
+        <c:axId val="-1263659696"/>
       </c:barChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -831,188 +855,221 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sayfa1!$A$14:$A$73</c:f>
+              <c:f>Sayfa1!$A$4:$A$74</c:f>
               <c:strCache>
-                <c:ptCount val="60"/>
+                <c:ptCount val="71"/>
                 <c:pt idx="0">
+                  <c:v>DAY2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>DAY3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>DAY4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>DAY5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>DAY6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>DAY7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>DAY8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>DAY9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>DAY10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>DAY11</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>DAY12</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="11">
                   <c:v>DAY13</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="12">
                   <c:v>DAY14</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="13">
                   <c:v>DAY15</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="14">
                   <c:v>DAY16</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="15">
                   <c:v>DAY17</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="16">
                   <c:v>DAY18</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="17">
                   <c:v>DAY19</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="18">
                   <c:v>DAY20</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="19">
                   <c:v>DAY21</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="20">
                   <c:v>DAY22</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="21">
                   <c:v>DAY23</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="22">
                   <c:v>DAY24</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="23">
                   <c:v>DAY25</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="24">
                   <c:v>DAY26</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="25">
                   <c:v>DAY27</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="26">
                   <c:v>DAY28</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="27">
                   <c:v>DAY29</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="28">
                   <c:v>DAY30</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="29">
                   <c:v>DAY31</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="30">
                   <c:v>DAY32</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="31">
                   <c:v>DAY33</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="32">
                   <c:v>DAY34</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="33">
                   <c:v>DAY35</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="34">
                   <c:v>DAY36</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="35">
                   <c:v>DAY37</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="36">
                   <c:v>DAY38</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="37">
                   <c:v>DAY39</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="38">
                   <c:v>DAY40</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="39">
                   <c:v>DAY41</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="40">
                   <c:v>DAY42</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="41">
                   <c:v>DAY43</c:v>
                 </c:pt>
-                <c:pt idx="32">
+                <c:pt idx="42">
                   <c:v>DAY44</c:v>
                 </c:pt>
-                <c:pt idx="33">
+                <c:pt idx="43">
                   <c:v>DAY45</c:v>
                 </c:pt>
-                <c:pt idx="34">
+                <c:pt idx="44">
                   <c:v>DAY46</c:v>
                 </c:pt>
-                <c:pt idx="35">
+                <c:pt idx="45">
                   <c:v>DAY47</c:v>
                 </c:pt>
-                <c:pt idx="36">
+                <c:pt idx="46">
                   <c:v>DAY48</c:v>
                 </c:pt>
-                <c:pt idx="37">
+                <c:pt idx="47">
                   <c:v>DAY49</c:v>
                 </c:pt>
-                <c:pt idx="38">
+                <c:pt idx="48">
                   <c:v>DAY50</c:v>
                 </c:pt>
-                <c:pt idx="39">
+                <c:pt idx="49">
                   <c:v>DAY51</c:v>
                 </c:pt>
-                <c:pt idx="40">
+                <c:pt idx="50">
                   <c:v>DAY52</c:v>
                 </c:pt>
-                <c:pt idx="41">
+                <c:pt idx="51">
                   <c:v>DAY53</c:v>
                 </c:pt>
-                <c:pt idx="42">
+                <c:pt idx="52">
                   <c:v>DAY54</c:v>
                 </c:pt>
-                <c:pt idx="43">
+                <c:pt idx="53">
                   <c:v>DAY55</c:v>
                 </c:pt>
-                <c:pt idx="44">
+                <c:pt idx="54">
                   <c:v>DAY56</c:v>
                 </c:pt>
-                <c:pt idx="45">
+                <c:pt idx="55">
                   <c:v>DAY57</c:v>
                 </c:pt>
-                <c:pt idx="46">
+                <c:pt idx="56">
                   <c:v>DAY58</c:v>
                 </c:pt>
-                <c:pt idx="47">
+                <c:pt idx="57">
                   <c:v>DAY59</c:v>
                 </c:pt>
-                <c:pt idx="48">
+                <c:pt idx="58">
                   <c:v>DAY60</c:v>
                 </c:pt>
-                <c:pt idx="49">
+                <c:pt idx="59">
                   <c:v>DAY61</c:v>
                 </c:pt>
-                <c:pt idx="50">
+                <c:pt idx="60">
                   <c:v>DAY62</c:v>
                 </c:pt>
-                <c:pt idx="51">
+                <c:pt idx="61">
                   <c:v>DAY63</c:v>
                 </c:pt>
-                <c:pt idx="52">
+                <c:pt idx="62">
                   <c:v>DAY64</c:v>
                 </c:pt>
-                <c:pt idx="53">
+                <c:pt idx="63">
                   <c:v>DAY65</c:v>
                 </c:pt>
-                <c:pt idx="54">
+                <c:pt idx="64">
                   <c:v>DAY66</c:v>
                 </c:pt>
-                <c:pt idx="55">
+                <c:pt idx="65">
                   <c:v>DAY67</c:v>
                 </c:pt>
-                <c:pt idx="56">
+                <c:pt idx="66">
                   <c:v>DAY68</c:v>
                 </c:pt>
-                <c:pt idx="57">
+                <c:pt idx="67">
                   <c:v>DAY69</c:v>
                 </c:pt>
-                <c:pt idx="58">
+                <c:pt idx="68">
                   <c:v>DAY70</c:v>
                 </c:pt>
-                <c:pt idx="59">
+                <c:pt idx="69">
                   <c:v>DAY71</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>DAY72</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1181,6 +1238,27 @@
                 </c:pt>
                 <c:pt idx="52">
                   <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1220,188 +1298,221 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sayfa1!$A$14:$A$73</c:f>
+              <c:f>Sayfa1!$A$4:$A$74</c:f>
               <c:strCache>
-                <c:ptCount val="60"/>
+                <c:ptCount val="71"/>
                 <c:pt idx="0">
+                  <c:v>DAY2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>DAY3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>DAY4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>DAY5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>DAY6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>DAY7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>DAY8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>DAY9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>DAY10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>DAY11</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>DAY12</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="11">
                   <c:v>DAY13</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="12">
                   <c:v>DAY14</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="13">
                   <c:v>DAY15</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="14">
                   <c:v>DAY16</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="15">
                   <c:v>DAY17</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="16">
                   <c:v>DAY18</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="17">
                   <c:v>DAY19</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="18">
                   <c:v>DAY20</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="19">
                   <c:v>DAY21</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="20">
                   <c:v>DAY22</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="21">
                   <c:v>DAY23</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="22">
                   <c:v>DAY24</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="23">
                   <c:v>DAY25</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="24">
                   <c:v>DAY26</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="25">
                   <c:v>DAY27</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="26">
                   <c:v>DAY28</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="27">
                   <c:v>DAY29</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="28">
                   <c:v>DAY30</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="29">
                   <c:v>DAY31</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="30">
                   <c:v>DAY32</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="31">
                   <c:v>DAY33</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="32">
                   <c:v>DAY34</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="33">
                   <c:v>DAY35</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="34">
                   <c:v>DAY36</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="35">
                   <c:v>DAY37</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="36">
                   <c:v>DAY38</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="37">
                   <c:v>DAY39</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="38">
                   <c:v>DAY40</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="39">
                   <c:v>DAY41</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="40">
                   <c:v>DAY42</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="41">
                   <c:v>DAY43</c:v>
                 </c:pt>
-                <c:pt idx="32">
+                <c:pt idx="42">
                   <c:v>DAY44</c:v>
                 </c:pt>
-                <c:pt idx="33">
+                <c:pt idx="43">
                   <c:v>DAY45</c:v>
                 </c:pt>
-                <c:pt idx="34">
+                <c:pt idx="44">
                   <c:v>DAY46</c:v>
                 </c:pt>
-                <c:pt idx="35">
+                <c:pt idx="45">
                   <c:v>DAY47</c:v>
                 </c:pt>
-                <c:pt idx="36">
+                <c:pt idx="46">
                   <c:v>DAY48</c:v>
                 </c:pt>
-                <c:pt idx="37">
+                <c:pt idx="47">
                   <c:v>DAY49</c:v>
                 </c:pt>
-                <c:pt idx="38">
+                <c:pt idx="48">
                   <c:v>DAY50</c:v>
                 </c:pt>
-                <c:pt idx="39">
+                <c:pt idx="49">
                   <c:v>DAY51</c:v>
                 </c:pt>
-                <c:pt idx="40">
+                <c:pt idx="50">
                   <c:v>DAY52</c:v>
                 </c:pt>
-                <c:pt idx="41">
+                <c:pt idx="51">
                   <c:v>DAY53</c:v>
                 </c:pt>
-                <c:pt idx="42">
+                <c:pt idx="52">
                   <c:v>DAY54</c:v>
                 </c:pt>
-                <c:pt idx="43">
+                <c:pt idx="53">
                   <c:v>DAY55</c:v>
                 </c:pt>
-                <c:pt idx="44">
+                <c:pt idx="54">
                   <c:v>DAY56</c:v>
                 </c:pt>
-                <c:pt idx="45">
+                <c:pt idx="55">
                   <c:v>DAY57</c:v>
                 </c:pt>
-                <c:pt idx="46">
+                <c:pt idx="56">
                   <c:v>DAY58</c:v>
                 </c:pt>
-                <c:pt idx="47">
+                <c:pt idx="57">
                   <c:v>DAY59</c:v>
                 </c:pt>
-                <c:pt idx="48">
+                <c:pt idx="58">
                   <c:v>DAY60</c:v>
                 </c:pt>
-                <c:pt idx="49">
+                <c:pt idx="59">
                   <c:v>DAY61</c:v>
                 </c:pt>
-                <c:pt idx="50">
+                <c:pt idx="60">
                   <c:v>DAY62</c:v>
                 </c:pt>
-                <c:pt idx="51">
+                <c:pt idx="61">
                   <c:v>DAY63</c:v>
                 </c:pt>
-                <c:pt idx="52">
+                <c:pt idx="62">
                   <c:v>DAY64</c:v>
                 </c:pt>
-                <c:pt idx="53">
+                <c:pt idx="63">
                   <c:v>DAY65</c:v>
                 </c:pt>
-                <c:pt idx="54">
+                <c:pt idx="64">
                   <c:v>DAY66</c:v>
                 </c:pt>
-                <c:pt idx="55">
+                <c:pt idx="65">
                   <c:v>DAY67</c:v>
                 </c:pt>
-                <c:pt idx="56">
+                <c:pt idx="66">
                   <c:v>DAY68</c:v>
                 </c:pt>
-                <c:pt idx="57">
+                <c:pt idx="67">
                   <c:v>DAY69</c:v>
                 </c:pt>
-                <c:pt idx="58">
+                <c:pt idx="68">
                   <c:v>DAY70</c:v>
                 </c:pt>
-                <c:pt idx="59">
+                <c:pt idx="69">
                   <c:v>DAY71</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>DAY72</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1630,188 +1741,221 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sayfa1!$A$14:$A$73</c:f>
+              <c:f>Sayfa1!$A$4:$A$74</c:f>
               <c:strCache>
-                <c:ptCount val="60"/>
+                <c:ptCount val="71"/>
                 <c:pt idx="0">
+                  <c:v>DAY2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>DAY3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>DAY4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>DAY5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>DAY6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>DAY7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>DAY8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>DAY9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>DAY10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>DAY11</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>DAY12</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="11">
                   <c:v>DAY13</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="12">
                   <c:v>DAY14</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="13">
                   <c:v>DAY15</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="14">
                   <c:v>DAY16</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="15">
                   <c:v>DAY17</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="16">
                   <c:v>DAY18</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="17">
                   <c:v>DAY19</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="18">
                   <c:v>DAY20</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="19">
                   <c:v>DAY21</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="20">
                   <c:v>DAY22</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="21">
                   <c:v>DAY23</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="22">
                   <c:v>DAY24</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="23">
                   <c:v>DAY25</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="24">
                   <c:v>DAY26</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="25">
                   <c:v>DAY27</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="26">
                   <c:v>DAY28</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="27">
                   <c:v>DAY29</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="28">
                   <c:v>DAY30</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="29">
                   <c:v>DAY31</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="30">
                   <c:v>DAY32</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="31">
                   <c:v>DAY33</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="32">
                   <c:v>DAY34</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="33">
                   <c:v>DAY35</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="34">
                   <c:v>DAY36</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="35">
                   <c:v>DAY37</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="36">
                   <c:v>DAY38</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="37">
                   <c:v>DAY39</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="38">
                   <c:v>DAY40</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="39">
                   <c:v>DAY41</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="40">
                   <c:v>DAY42</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="41">
                   <c:v>DAY43</c:v>
                 </c:pt>
-                <c:pt idx="32">
+                <c:pt idx="42">
                   <c:v>DAY44</c:v>
                 </c:pt>
-                <c:pt idx="33">
+                <c:pt idx="43">
                   <c:v>DAY45</c:v>
                 </c:pt>
-                <c:pt idx="34">
+                <c:pt idx="44">
                   <c:v>DAY46</c:v>
                 </c:pt>
-                <c:pt idx="35">
+                <c:pt idx="45">
                   <c:v>DAY47</c:v>
                 </c:pt>
-                <c:pt idx="36">
+                <c:pt idx="46">
                   <c:v>DAY48</c:v>
                 </c:pt>
-                <c:pt idx="37">
+                <c:pt idx="47">
                   <c:v>DAY49</c:v>
                 </c:pt>
-                <c:pt idx="38">
+                <c:pt idx="48">
                   <c:v>DAY50</c:v>
                 </c:pt>
-                <c:pt idx="39">
+                <c:pt idx="49">
                   <c:v>DAY51</c:v>
                 </c:pt>
-                <c:pt idx="40">
+                <c:pt idx="50">
                   <c:v>DAY52</c:v>
                 </c:pt>
-                <c:pt idx="41">
+                <c:pt idx="51">
                   <c:v>DAY53</c:v>
                 </c:pt>
-                <c:pt idx="42">
+                <c:pt idx="52">
                   <c:v>DAY54</c:v>
                 </c:pt>
-                <c:pt idx="43">
+                <c:pt idx="53">
                   <c:v>DAY55</c:v>
                 </c:pt>
-                <c:pt idx="44">
+                <c:pt idx="54">
                   <c:v>DAY56</c:v>
                 </c:pt>
-                <c:pt idx="45">
+                <c:pt idx="55">
                   <c:v>DAY57</c:v>
                 </c:pt>
-                <c:pt idx="46">
+                <c:pt idx="56">
                   <c:v>DAY58</c:v>
                 </c:pt>
-                <c:pt idx="47">
+                <c:pt idx="57">
                   <c:v>DAY59</c:v>
                 </c:pt>
-                <c:pt idx="48">
+                <c:pt idx="58">
                   <c:v>DAY60</c:v>
                 </c:pt>
-                <c:pt idx="49">
+                <c:pt idx="59">
                   <c:v>DAY61</c:v>
                 </c:pt>
-                <c:pt idx="50">
+                <c:pt idx="60">
                   <c:v>DAY62</c:v>
                 </c:pt>
-                <c:pt idx="51">
+                <c:pt idx="61">
                   <c:v>DAY63</c:v>
                 </c:pt>
-                <c:pt idx="52">
+                <c:pt idx="62">
                   <c:v>DAY64</c:v>
                 </c:pt>
-                <c:pt idx="53">
+                <c:pt idx="63">
                   <c:v>DAY65</c:v>
                 </c:pt>
-                <c:pt idx="54">
+                <c:pt idx="64">
                   <c:v>DAY66</c:v>
                 </c:pt>
-                <c:pt idx="55">
+                <c:pt idx="65">
                   <c:v>DAY67</c:v>
                 </c:pt>
-                <c:pt idx="56">
+                <c:pt idx="66">
                   <c:v>DAY68</c:v>
                 </c:pt>
-                <c:pt idx="57">
+                <c:pt idx="67">
                   <c:v>DAY69</c:v>
                 </c:pt>
-                <c:pt idx="58">
+                <c:pt idx="68">
                   <c:v>DAY70</c:v>
                 </c:pt>
-                <c:pt idx="59">
+                <c:pt idx="69">
                   <c:v>DAY71</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>DAY72</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1980,6 +2124,27 @@
                 </c:pt>
                 <c:pt idx="52">
                   <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2016,188 +2181,221 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Sayfa1!$A$14:$A$73</c:f>
+              <c:f>Sayfa1!$A$4:$A$74</c:f>
               <c:strCache>
-                <c:ptCount val="60"/>
+                <c:ptCount val="71"/>
                 <c:pt idx="0">
+                  <c:v>DAY2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>DAY3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>DAY4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>DAY5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>DAY6</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>DAY7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>DAY8</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>DAY9</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>DAY10</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>DAY11</c:v>
+                </c:pt>
+                <c:pt idx="10">
                   <c:v>DAY12</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="11">
                   <c:v>DAY13</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="12">
                   <c:v>DAY14</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="13">
                   <c:v>DAY15</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="14">
                   <c:v>DAY16</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="15">
                   <c:v>DAY17</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="16">
                   <c:v>DAY18</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="17">
                   <c:v>DAY19</c:v>
                 </c:pt>
-                <c:pt idx="8">
+                <c:pt idx="18">
                   <c:v>DAY20</c:v>
                 </c:pt>
-                <c:pt idx="9">
+                <c:pt idx="19">
                   <c:v>DAY21</c:v>
                 </c:pt>
-                <c:pt idx="10">
+                <c:pt idx="20">
                   <c:v>DAY22</c:v>
                 </c:pt>
-                <c:pt idx="11">
+                <c:pt idx="21">
                   <c:v>DAY23</c:v>
                 </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="22">
                   <c:v>DAY24</c:v>
                 </c:pt>
-                <c:pt idx="13">
+                <c:pt idx="23">
                   <c:v>DAY25</c:v>
                 </c:pt>
-                <c:pt idx="14">
+                <c:pt idx="24">
                   <c:v>DAY26</c:v>
                 </c:pt>
-                <c:pt idx="15">
+                <c:pt idx="25">
                   <c:v>DAY27</c:v>
                 </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="26">
                   <c:v>DAY28</c:v>
                 </c:pt>
-                <c:pt idx="17">
+                <c:pt idx="27">
                   <c:v>DAY29</c:v>
                 </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="28">
                   <c:v>DAY30</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="29">
                   <c:v>DAY31</c:v>
                 </c:pt>
-                <c:pt idx="20">
+                <c:pt idx="30">
                   <c:v>DAY32</c:v>
                 </c:pt>
-                <c:pt idx="21">
+                <c:pt idx="31">
                   <c:v>DAY33</c:v>
                 </c:pt>
-                <c:pt idx="22">
+                <c:pt idx="32">
                   <c:v>DAY34</c:v>
                 </c:pt>
-                <c:pt idx="23">
+                <c:pt idx="33">
                   <c:v>DAY35</c:v>
                 </c:pt>
-                <c:pt idx="24">
+                <c:pt idx="34">
                   <c:v>DAY36</c:v>
                 </c:pt>
-                <c:pt idx="25">
+                <c:pt idx="35">
                   <c:v>DAY37</c:v>
                 </c:pt>
-                <c:pt idx="26">
+                <c:pt idx="36">
                   <c:v>DAY38</c:v>
                 </c:pt>
-                <c:pt idx="27">
+                <c:pt idx="37">
                   <c:v>DAY39</c:v>
                 </c:pt>
-                <c:pt idx="28">
+                <c:pt idx="38">
                   <c:v>DAY40</c:v>
                 </c:pt>
-                <c:pt idx="29">
+                <c:pt idx="39">
                   <c:v>DAY41</c:v>
                 </c:pt>
-                <c:pt idx="30">
+                <c:pt idx="40">
                   <c:v>DAY42</c:v>
                 </c:pt>
-                <c:pt idx="31">
+                <c:pt idx="41">
                   <c:v>DAY43</c:v>
                 </c:pt>
-                <c:pt idx="32">
+                <c:pt idx="42">
                   <c:v>DAY44</c:v>
                 </c:pt>
-                <c:pt idx="33">
+                <c:pt idx="43">
                   <c:v>DAY45</c:v>
                 </c:pt>
-                <c:pt idx="34">
+                <c:pt idx="44">
                   <c:v>DAY46</c:v>
                 </c:pt>
-                <c:pt idx="35">
+                <c:pt idx="45">
                   <c:v>DAY47</c:v>
                 </c:pt>
-                <c:pt idx="36">
+                <c:pt idx="46">
                   <c:v>DAY48</c:v>
                 </c:pt>
-                <c:pt idx="37">
+                <c:pt idx="47">
                   <c:v>DAY49</c:v>
                 </c:pt>
-                <c:pt idx="38">
+                <c:pt idx="48">
                   <c:v>DAY50</c:v>
                 </c:pt>
-                <c:pt idx="39">
+                <c:pt idx="49">
                   <c:v>DAY51</c:v>
                 </c:pt>
-                <c:pt idx="40">
+                <c:pt idx="50">
                   <c:v>DAY52</c:v>
                 </c:pt>
-                <c:pt idx="41">
+                <c:pt idx="51">
                   <c:v>DAY53</c:v>
                 </c:pt>
-                <c:pt idx="42">
+                <c:pt idx="52">
                   <c:v>DAY54</c:v>
                 </c:pt>
-                <c:pt idx="43">
+                <c:pt idx="53">
                   <c:v>DAY55</c:v>
                 </c:pt>
-                <c:pt idx="44">
+                <c:pt idx="54">
                   <c:v>DAY56</c:v>
                 </c:pt>
-                <c:pt idx="45">
+                <c:pt idx="55">
                   <c:v>DAY57</c:v>
                 </c:pt>
-                <c:pt idx="46">
+                <c:pt idx="56">
                   <c:v>DAY58</c:v>
                 </c:pt>
-                <c:pt idx="47">
+                <c:pt idx="57">
                   <c:v>DAY59</c:v>
                 </c:pt>
-                <c:pt idx="48">
+                <c:pt idx="58">
                   <c:v>DAY60</c:v>
                 </c:pt>
-                <c:pt idx="49">
+                <c:pt idx="59">
                   <c:v>DAY61</c:v>
                 </c:pt>
-                <c:pt idx="50">
+                <c:pt idx="60">
                   <c:v>DAY62</c:v>
                 </c:pt>
-                <c:pt idx="51">
+                <c:pt idx="61">
                   <c:v>DAY63</c:v>
                 </c:pt>
-                <c:pt idx="52">
+                <c:pt idx="62">
                   <c:v>DAY64</c:v>
                 </c:pt>
-                <c:pt idx="53">
+                <c:pt idx="63">
                   <c:v>DAY65</c:v>
                 </c:pt>
-                <c:pt idx="54">
+                <c:pt idx="64">
                   <c:v>DAY66</c:v>
                 </c:pt>
-                <c:pt idx="55">
+                <c:pt idx="65">
                   <c:v>DAY67</c:v>
                 </c:pt>
-                <c:pt idx="56">
+                <c:pt idx="66">
                   <c:v>DAY68</c:v>
                 </c:pt>
-                <c:pt idx="57">
+                <c:pt idx="67">
                   <c:v>DAY69</c:v>
                 </c:pt>
-                <c:pt idx="58">
+                <c:pt idx="68">
                   <c:v>DAY70</c:v>
                 </c:pt>
-                <c:pt idx="59">
+                <c:pt idx="69">
                   <c:v>DAY71</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>DAY72</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -2231,11 +2429,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="439814576"/>
-        <c:axId val="439806960"/>
+        <c:axId val="-1263664048"/>
+        <c:axId val="-1263659696"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="439814576"/>
+        <c:axId val="-1263664048"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2278,7 +2476,7 @@
             <a:endParaRPr lang="tr-TR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="439806960"/>
+        <c:crossAx val="-1263659696"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2286,7 +2484,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="439806960"/>
+        <c:axId val="-1263659696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2323,7 +2521,7 @@
             <a:endParaRPr lang="tr-TR"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="439814576"/>
+        <c:crossAx val="-1263664048"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2337,6 +2535,10 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:legendEntry>
+        <c:idx val="4"/>
+        <c:delete val="1"/>
+      </c:legendEntry>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -2967,7 +3169,7 @@
         <xdr:cNvPr id="2" name="Grafik 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3251,10 +3453,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:F73"/>
+  <dimension ref="A2:F74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F63" sqref="F63"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4374,56 +4576,136 @@
       <c r="A67" t="s">
         <v>68</v>
       </c>
+      <c r="B67">
+        <v>0</v>
+      </c>
+      <c r="C67">
+        <v>24</v>
+      </c>
       <c r="D67">
         <v>7</v>
+      </c>
+      <c r="E67">
+        <v>24</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>69</v>
       </c>
+      <c r="B68">
+        <v>2</v>
+      </c>
+      <c r="C68">
+        <v>18</v>
+      </c>
       <c r="D68">
         <v>6</v>
+      </c>
+      <c r="E68">
+        <v>16</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>70</v>
       </c>
+      <c r="B69">
+        <v>0</v>
+      </c>
+      <c r="C69">
+        <v>18</v>
+      </c>
       <c r="D69">
         <v>5</v>
+      </c>
+      <c r="E69">
+        <v>16</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>71</v>
       </c>
+      <c r="B70">
+        <v>4</v>
+      </c>
+      <c r="C70">
+        <v>14</v>
+      </c>
       <c r="D70">
         <v>4</v>
+      </c>
+      <c r="E70">
+        <v>13</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>72</v>
       </c>
+      <c r="B71">
+        <v>6</v>
+      </c>
+      <c r="C71">
+        <v>8</v>
+      </c>
       <c r="D71">
         <v>3</v>
+      </c>
+      <c r="E71">
+        <v>8</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>73</v>
       </c>
+      <c r="B72">
+        <v>4</v>
+      </c>
+      <c r="C72">
+        <v>4</v>
+      </c>
       <c r="D72">
         <v>2</v>
+      </c>
+      <c r="E72">
+        <v>4</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>74</v>
       </c>
+      <c r="B73">
+        <v>3</v>
+      </c>
+      <c r="C73">
+        <v>1</v>
+      </c>
       <c r="D73">
         <v>1</v>
+      </c>
+      <c r="E73">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>75</v>
+      </c>
+      <c r="B74">
+        <v>1</v>
+      </c>
+      <c r="C74">
+        <v>0</v>
+      </c>
+      <c r="D74">
+        <v>0</v>
+      </c>
+      <c r="E74">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>